<commit_message>
added sheet with new troy results
git-svn-id: file://localhost/tmp/svn2git/svn@4909 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/performance.xlsx
+++ b/papers/troy/pstar/perf/performance.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="3820" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="File Transfer" sheetId="1" r:id="rId1"/>
     <sheet name="SubJob Throughput" sheetId="2" r:id="rId2"/>
+    <sheet name="TROY" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Throughput (in MB/s)</t>
   </si>
@@ -51,6 +52,42 @@
   </si>
   <si>
     <t>Percent of GridFTP performance</t>
+  </si>
+  <si>
+    <t>Number of tasks</t>
+  </si>
+  <si>
+    <t>Number of threads per task</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>painter</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>matching</t>
+  </si>
+  <si>
+    <t>TTC</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>BJ-SAGA</t>
+  </si>
+  <si>
+    <t>BJ-Diane</t>
+  </si>
+  <si>
+    <t>BJ-SAGA, BJ-Diane</t>
+  </si>
+  <si>
+    <t>Number of cores</t>
   </si>
 </sst>
 </file>
@@ -58,9 +95,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm:ss.0;@"/>
+    <numFmt numFmtId="164" formatCode="mm:ss.0;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +136,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,8 +161,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -144,53 +198,66 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="26" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="26">
-    <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="31">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 1" xfId="26" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -521,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -535,15 +602,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="45">
       <c r="A2" s="1" t="s">
@@ -579,14 +646,14 @@
         <f>($A3/1024/1024)/(B3*24*60*60)</f>
         <v>11.606033611387623</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>9.6579861111111096E-4</v>
       </c>
       <c r="E3" s="3">
         <f>($A3/1024/1024)/(D3*24*60*60)</f>
         <v>13.704007258630369</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <f>C3/E3</f>
         <v>0.84690801692902595</v>
       </c>
@@ -598,21 +665,21 @@
       <c r="A4">
         <v>1199079042</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>1.0543634259259258E-3</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:C7" si="0">($A4/1024/1024)/(B4*24*60*60)</f>
         <v>12.552892913009334</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>2.5984953703703706E-4</v>
       </c>
       <c r="E4" s="3">
         <f>($A4/1024/1024)/(D4*24*60*60)</f>
         <v>50.934518983404352</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <f t="shared" ref="F4:F7" si="1">C4/E4</f>
         <v>0.24645158457468416</v>
       </c>
@@ -624,21 +691,21 @@
       <c r="A5">
         <v>1199079042</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>1.0416666666666667E-3</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>12.705898729960124</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>2.54537037037037E-4</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ref="E5:E7" si="2">($A5/1024/1024)/(D5*24*60*60)</f>
         <v>51.997584835231507</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <f t="shared" si="1"/>
         <v>0.24435555555555552</v>
       </c>
@@ -650,21 +717,21 @@
       <c r="A6">
         <v>1199079042</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>9.5180555555555556E-4</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>13.905477962162692</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>1.7192129629629629E-4</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="2"/>
         <v>76.984710225960086</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f t="shared" si="1"/>
         <v>0.18062648961525365</v>
       </c>
@@ -676,21 +743,21 @@
       <c r="A7">
         <v>1199079042</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>9.5292824074074073E-4</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>13.889095328682437</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>1.5527777777777778E-4</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="2"/>
         <v>85.236351050716394</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>0.16294802812966852</v>
       </c>
@@ -728,4 +795,118 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B6:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:8" s="9" customFormat="1" ht="58" thickBot="1">
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="16" thickTop="1">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
results including qb and painter
git-svn-id: file://localhost/tmp/svn2git/svn@4944 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/performance.xlsx
+++ b/papers/troy/pstar/perf/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="File Transfer" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>Throughput (in MB/s)</t>
   </si>
@@ -72,9 +72,6 @@
     <t>matching</t>
   </si>
   <si>
-    <t>TTC</t>
-  </si>
-  <si>
     <t>Backend</t>
   </si>
   <si>
@@ -88,6 +85,37 @@
   </si>
   <si>
     <t>Number of cores</t>
+  </si>
+  <si>
+    <t>TTC(only matching)</t>
+  </si>
+  <si>
+    <t>error with four workers per node</t>
+  </si>
+  <si>
+    <t>4, 4</t>
+  </si>
+  <si>
+    <t>qb</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>real time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12m11.266s
+</t>
+  </si>
+  <si>
+    <t>8m17.946s</t>
+  </si>
+  <si>
+    <t>tasks/node</t>
+  </si>
+  <si>
+    <t>10m17.069s</t>
   </si>
 </sst>
 </file>
@@ -171,7 +199,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -203,8 +231,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -216,17 +252,23 @@
     </xf>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="26" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="26" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="26" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -241,6 +283,10 @@
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="26" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -256,6 +302,10 @@
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -602,14 +652,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="45">
@@ -799,44 +849,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:H9"/>
+  <dimension ref="A6:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:8" s="9" customFormat="1" ht="58" thickBot="1">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="58" thickBot="1">
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" thickTop="1">
+      <c r="B7" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="16" thickTop="1">
-      <c r="B7" t="s">
-        <v>18</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -857,9 +908,9 @@
         <v>529</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="1:11">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -877,12 +928,15 @@
         <v>15</v>
       </c>
       <c r="H8">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
+        <v>941</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -898,6 +952,227 @@
       </c>
       <c r="G9" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="58" thickBot="1">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="16" thickTop="1">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>529</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>542</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>545</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="58" thickBot="1">
+      <c r="B25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="16" thickTop="1">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26">
+        <v>494</v>
+      </c>
+      <c r="J26" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="45">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27">
+        <v>485</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28">
+        <v>521</v>
+      </c>
+      <c r="J28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>